<commit_message>
debugging for stock price through api
</commit_message>
<xml_diff>
--- a/electron/data/summary.xlsx
+++ b/electron/data/summary.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -490,7 +490,7 @@
         <v>20.49005816087204</v>
       </c>
       <c r="M2">
-        <v>10.441419096404312</v>
+        <v>10.229247324523367</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -537,7 +537,7 @@
         <v>82.18788715184354</v>
       </c>
       <c r="M3">
-        <v>36.89221215791324</v>
+        <v>36.14255486038673</v>
       </c>
       <c r="N3">
         <v>8611.5</v>
@@ -584,7 +584,7 @@
         <v>18.020709116025362</v>
       </c>
       <c r="M4">
-        <v>8.768655540859772</v>
+        <v>8.590474666599244</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -631,7 +631,7 @@
         <v>11.700789324007905</v>
       </c>
       <c r="M5">
-        <v>24.675561129726773</v>
+        <v>24.174148680067166</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>23.24930626575447</v>
       </c>
       <c r="M6">
-        <v>7.46056483400597</v>
+        <v>7.308964630484898</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -725,7 +725,7 @@
         <v>15.12022590490317</v>
       </c>
       <c r="M7">
-        <v>3.629647975807912</v>
+        <v>3.555892786477714</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>29.909408081419507</v>
       </c>
       <c r="M8">
-        <v>1.2302168064463443</v>
+        <v>1.2052185492926475</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -819,7 +819,7 @@
         <v>18.368101346600067</v>
       </c>
       <c r="M9">
-        <v>3.5581483888619454</v>
+        <v>3.48584608576407</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>6.014634395689007</v>
       </c>
       <c r="M10">
-        <v>1.3859659383426939</v>
+        <v>1.3578028269696363</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>NaN</v>
       </c>
       <c r="M11">
-        <v>1.8273463717737144</v>
+        <v>1.7902143197068687</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -960,7 +960,7 @@
         <v>7.750519766484215</v>
       </c>
       <c r="M12">
-        <v>0.10785869751756595</v>
+        <v>0.10566698672099871</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1007,18 +1007,65 @@
         <v>0.35463319910200686</v>
       </c>
       <c r="M13">
-        <v>0.022403062339764714</v>
+        <v>0.02194782753036759</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>NESTLE</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Equity</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Nestle Pakistan Limited</v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v>FOOD &amp; PERSONAL CARE PRODUCTS</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>5008.63</v>
+      </c>
+      <c r="H14">
+        <v>5008.63</v>
+      </c>
+      <c r="I14" t="str">
+        <v>8,412.42</v>
+      </c>
+      <c r="J14">
+        <v>-32.84</v>
+      </c>
+      <c r="K14" t="str">
+        <v>(-0.39%)</v>
+      </c>
+      <c r="L14">
+        <v>NaN</v>
+      </c>
+      <c r="M14">
+        <v>2.032020455476297</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>